<commit_message>
+Update Added more comments
</commit_message>
<xml_diff>
--- a/Calc Timer.xlsx
+++ b/Calc Timer.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C3A49B-0FA7-4987-B139-D8CDC95A39CA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E689E5-AA91-4FAE-8F86-C7588532C720}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>Divider N</t>
   </si>
@@ -81,7 +81,17 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -368,18 +378,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:E8"/>
+  <dimension ref="B3:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="54.7109375" customWidth="1"/>
+    <col min="9" max="9" width="33.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -392,8 +403,20 @@
       <c r="E3" s="1">
         <v>16000000</v>
       </c>
+      <c r="H3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="1">
+        <v>16000000</v>
+      </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -407,8 +430,21 @@
       <c r="E4" s="1">
         <v>3.4250000000000001E-3</v>
       </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2">
+        <f>($K$3*$K$4)/(2*H4)-1</f>
+        <v>11039</v>
+      </c>
+      <c r="J4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1.3799999999999999E-3</v>
+      </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>8</v>
       </c>
@@ -416,8 +452,15 @@
         <f>($E$3*$E$4)/(2*B5)-1</f>
         <v>3424</v>
       </c>
+      <c r="H5">
+        <v>8</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" ref="I5:I8" si="0">($K$3*$K$4)/(2*H5)-1</f>
+        <v>1379</v>
+      </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>64</v>
       </c>
@@ -425,8 +468,15 @@
         <f>($E$3*$E$4)/(2*B6)-1</f>
         <v>427.125</v>
       </c>
+      <c r="H6">
+        <v>64</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="0"/>
+        <v>171.5</v>
+      </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>256</v>
       </c>
@@ -434,8 +484,15 @@
         <f>($E$3*$E$4)/(2*B7)-1</f>
         <v>106.03125</v>
       </c>
+      <c r="H7">
+        <v>256</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="0"/>
+        <v>42.125</v>
+      </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>1024</v>
       </c>
@@ -443,13 +500,26 @@
         <f>($E$3*$E$4)/(2*B8)-1</f>
         <v>25.7578125</v>
       </c>
+      <c r="H8">
+        <v>1024</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="0"/>
+        <v>9.78125</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C4:C8">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+      <formula>65536</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:I8">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>65536</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>